<commit_message>
Update number of RED units `nr` in data file sheet stack_param
</commit_message>
<xml_diff>
--- a/gdplib/reverse_electrodialysis/data.xlsx
+++ b/gdplib/reverse_electrodialysis/data.xlsx
@@ -502,7 +502,7 @@
     <col min="9" max="9" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="8" t="s">
         <v>6</v>
       </c>
@@ -638,7 +638,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="8">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B2" s="2">
         <v>0.456</v>

</xml_diff>